<commit_message>
Studienarbeit aktualisiert: Anpassungen an der Schriftart, Verzeichnisbeschreibung und verschiedene Dateianpassungen vorgenommen
</commit_message>
<xml_diff>
--- a/Model_Doku_Master_STA2.xlsx
+++ b/Model_Doku_Master_STA2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreasbraig/Documents/VSCode/DHBWMA_HHAT_Image-Classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C73B87B-88A2-1048-8AB5-F1779DD6EA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{55AAAABA-1822-B849-83DC-B7624F5A5218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11480" yWindow="5500" windowWidth="28240" windowHeight="17240" xr2:uid="{D564533F-BAE4-C643-AF37-CB06E8464E9E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27180" xr2:uid="{D564533F-BAE4-C643-AF37-CB06E8464E9E}"/>
   </bookViews>
   <sheets>
     <sheet name="model30_NEWNET" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>epoch</t>
   </si>
@@ -32,138 +32,6 @@
   </si>
   <si>
     <t>timestamp</t>
-  </si>
-  <si>
-    <t>0.6246907114982605</t>
-  </si>
-  <si>
-    <t>0.6916666626930237</t>
-  </si>
-  <si>
-    <t>0.6071696281433105</t>
-  </si>
-  <si>
-    <t>0.7041666507720947</t>
-  </si>
-  <si>
-    <t>0.6097280383110046</t>
-  </si>
-  <si>
-    <t>0.6085821390151978</t>
-  </si>
-  <si>
-    <t>0.7166666388511658</t>
-  </si>
-  <si>
-    <t>0.6337814927101135</t>
-  </si>
-  <si>
-    <t>0.6791666746139526</t>
-  </si>
-  <si>
-    <t>0.6396594047546387</t>
-  </si>
-  <si>
-    <t>0.6177122592926025</t>
-  </si>
-  <si>
-    <t>0.5973427295684814</t>
-  </si>
-  <si>
-    <t>0.5990378260612488</t>
-  </si>
-  <si>
-    <t>0.6177143454551697</t>
-  </si>
-  <si>
-    <t>0.6277469992637634</t>
-  </si>
-  <si>
-    <t>0.5959972739219666</t>
-  </si>
-  <si>
-    <t>0.6179362535476685</t>
-  </si>
-  <si>
-    <t>0.5966927409172058</t>
-  </si>
-  <si>
-    <t>0.6176442503929138</t>
-  </si>
-  <si>
-    <t>0.6170782446861267</t>
-  </si>
-  <si>
-    <t>0.605648398399353</t>
-  </si>
-  <si>
-    <t>0.5933019518852234</t>
-  </si>
-  <si>
-    <t>0.6060376763343811</t>
-  </si>
-  <si>
-    <t>0.4885360896587372</t>
-  </si>
-  <si>
-    <t>0.4182145595550537</t>
-  </si>
-  <si>
-    <t>0.8083333373069763</t>
-  </si>
-  <si>
-    <t>0.2975287139415741</t>
-  </si>
-  <si>
-    <t>0.9166666865348816</t>
-  </si>
-  <si>
-    <t>0.16046765446662903</t>
-  </si>
-  <si>
-    <t>0.9125000238418579</t>
-  </si>
-  <si>
-    <t>0.10482966899871826</t>
-  </si>
-  <si>
-    <t>0.9583333134651184</t>
-  </si>
-  <si>
-    <t>0.07551702857017517</t>
-  </si>
-  <si>
-    <t>0.9750000238418579</t>
-  </si>
-  <si>
-    <t>0.030826391652226448</t>
-  </si>
-  <si>
-    <t>0.9833333492279053</t>
-  </si>
-  <si>
-    <t>0.008165192790329456</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>0.03392034396529198</t>
-  </si>
-  <si>
-    <t>0.987500011920929</t>
-  </si>
-  <si>
-    <t>0.1600445806980133</t>
-  </si>
-  <si>
-    <t>0.9208333492279053</t>
-  </si>
-  <si>
-    <t>0.2865907549858093</t>
-  </si>
-  <si>
-    <t>date</t>
   </si>
 </sst>
 </file>
@@ -707,6 +575,1401 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="2000" b="1"/>
+              <a:t>Trainigshistorie PyTorch Model</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>model30_NEWNET!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>epoch_loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>model30_NEWNET!$A$2:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>model30_NEWNET!$B$2:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.62469071149826005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.60716962814330999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.60972803831100397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.60858213901519698</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63378149271011297</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.63965940475463801</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.61771225929260198</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.597342729568481</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.599037826061248</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.61771434545516901</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.62774699926376298</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.595997273921966</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.61793625354766801</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.59669274091720503</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.61764425039291304</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.61707824468612604</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.60564839839935303</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.59330195188522294</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.60603767633438099</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.48853608965873702</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.41821455955505299</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.29752871394157399</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.160467654466629</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.104829668998718</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.5517028570175102E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.0826391652226399E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.1651927903294494E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.3920343965291901E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.160044580698013</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.28659075498580899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E80B-0A4C-BBBD-31CFDD932026}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>model30_NEWNET!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>epoch_acc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>model30_NEWNET!$A$2:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>model30_NEWNET!$C$2:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.69166666269302302</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70416665077209395</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70416665077209395</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.71666663885116499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67916667461395197</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69166666269302302</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69166666269302302</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.71666663885116499</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.71666663885116499</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.69166666269302302</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.67916667461395197</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.71666663885116499</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.69166666269302302</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.71666663885116499</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.69166666269302302</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.69166666269302302</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.70416665077209395</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.71666663885116499</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.69166666269302302</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.70416665077209395</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.80833333730697599</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.91666668653488104</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.91250002384185702</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.95833331346511796</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.97500002384185702</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98333334922790505</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.98750001192092896</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.92083334922790505</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.92083334922790505</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E80B-0A4C-BBBD-31CFDD932026}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="639810640"/>
+        <c:axId val="639812368"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="639810640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1400" b="1"/>
+                  <a:t>Epochen</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.88506364867898324"/>
+              <c:y val="0.93032407407407391"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="639812368"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="639812368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="639810640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5768AE0-1B80-2D3A-E203-8CCA710185AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1028,8 +2291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50263B4-DD00-C44E-8074-4A680FFC1D62}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1052,7 +2315,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1062,11 +2325,11 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+      <c r="B2">
+        <v>0.62469071149826005</v>
+      </c>
+      <c r="C2">
+        <v>0.69166666269302302</v>
       </c>
       <c r="D2" s="1">
         <v>45718</v>
@@ -1079,11 +2342,11 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
+      <c r="B3">
+        <v>0.60716962814330999</v>
+      </c>
+      <c r="C3">
+        <v>0.70416665077209395</v>
       </c>
       <c r="D3" s="1">
         <v>45718</v>
@@ -1096,11 +2359,11 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+      <c r="B4">
+        <v>0.60972803831100397</v>
+      </c>
+      <c r="C4">
+        <v>0.70416665077209395</v>
       </c>
       <c r="D4" s="1">
         <v>45718</v>
@@ -1113,11 +2376,11 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
+      <c r="B5">
+        <v>0.60858213901519698</v>
+      </c>
+      <c r="C5">
+        <v>0.71666663885116499</v>
       </c>
       <c r="D5" s="1">
         <v>45718</v>
@@ -1130,11 +2393,11 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
+      <c r="B6">
+        <v>0.63378149271011297</v>
+      </c>
+      <c r="C6">
+        <v>0.67916667461395197</v>
       </c>
       <c r="D6" s="1">
         <v>45718</v>
@@ -1147,11 +2410,11 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
+      <c r="B7">
+        <v>0.63965940475463801</v>
+      </c>
+      <c r="C7">
+        <v>0.69166666269302302</v>
       </c>
       <c r="D7" s="1">
         <v>45718</v>
@@ -1164,11 +2427,11 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
+      <c r="B8">
+        <v>0.61771225929260198</v>
+      </c>
+      <c r="C8">
+        <v>0.69166666269302302</v>
       </c>
       <c r="D8" s="1">
         <v>45718</v>
@@ -1181,11 +2444,11 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
+      <c r="B9">
+        <v>0.597342729568481</v>
+      </c>
+      <c r="C9">
+        <v>0.71666663885116499</v>
       </c>
       <c r="D9" s="1">
         <v>45718</v>
@@ -1198,11 +2461,11 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
+      <c r="B10">
+        <v>0.599037826061248</v>
+      </c>
+      <c r="C10">
+        <v>0.71666663885116499</v>
       </c>
       <c r="D10" s="1">
         <v>45718</v>
@@ -1215,11 +2478,11 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
+      <c r="B11">
+        <v>0.61771434545516901</v>
+      </c>
+      <c r="C11">
+        <v>0.69166666269302302</v>
       </c>
       <c r="D11" s="1">
         <v>45718</v>
@@ -1232,11 +2495,11 @@
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
+      <c r="B12">
+        <v>0.62774699926376298</v>
+      </c>
+      <c r="C12">
+        <v>0.67916667461395197</v>
       </c>
       <c r="D12" s="1">
         <v>45718</v>
@@ -1249,11 +2512,11 @@
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
+      <c r="B13">
+        <v>0.595997273921966</v>
+      </c>
+      <c r="C13">
+        <v>0.71666663885116499</v>
       </c>
       <c r="D13" s="1">
         <v>45718</v>
@@ -1266,11 +2529,11 @@
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
+      <c r="B14">
+        <v>0.61793625354766801</v>
+      </c>
+      <c r="C14">
+        <v>0.69166666269302302</v>
       </c>
       <c r="D14" s="1">
         <v>45718</v>
@@ -1283,11 +2546,11 @@
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
+      <c r="B15">
+        <v>0.59669274091720503</v>
+      </c>
+      <c r="C15">
+        <v>0.71666663885116499</v>
       </c>
       <c r="D15" s="1">
         <v>45718</v>
@@ -1300,11 +2563,11 @@
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
+      <c r="B16">
+        <v>0.61764425039291304</v>
+      </c>
+      <c r="C16">
+        <v>0.69166666269302302</v>
       </c>
       <c r="D16" s="1">
         <v>45718</v>
@@ -1317,11 +2580,11 @@
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
+      <c r="B17">
+        <v>0.61707824468612604</v>
+      </c>
+      <c r="C17">
+        <v>0.69166666269302302</v>
       </c>
       <c r="D17" s="1">
         <v>45718</v>
@@ -1334,11 +2597,11 @@
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
+      <c r="B18">
+        <v>0.60564839839935303</v>
+      </c>
+      <c r="C18">
+        <v>0.70416665077209395</v>
       </c>
       <c r="D18" s="1">
         <v>45718</v>
@@ -1351,11 +2614,11 @@
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
+      <c r="B19">
+        <v>0.59330195188522294</v>
+      </c>
+      <c r="C19">
+        <v>0.71666663885116499</v>
       </c>
       <c r="D19" s="1">
         <v>45718</v>
@@ -1368,11 +2631,11 @@
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
+      <c r="B20">
+        <v>0.60603767633438099</v>
+      </c>
+      <c r="C20">
+        <v>0.69166666269302302</v>
       </c>
       <c r="D20" s="1">
         <v>45718</v>
@@ -1385,11 +2648,11 @@
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
+      <c r="B21">
+        <v>0.48853608965873702</v>
+      </c>
+      <c r="C21">
+        <v>0.70416665077209395</v>
       </c>
       <c r="D21" s="1">
         <v>45718</v>
@@ -1402,11 +2665,11 @@
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" t="s">
-        <v>29</v>
+      <c r="B22">
+        <v>0.41821455955505299</v>
+      </c>
+      <c r="C22">
+        <v>0.80833333730697599</v>
       </c>
       <c r="D22" s="1">
         <v>45718</v>
@@ -1419,11 +2682,11 @@
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" t="s">
-        <v>31</v>
+      <c r="B23">
+        <v>0.29752871394157399</v>
+      </c>
+      <c r="C23">
+        <v>0.91666668653488104</v>
       </c>
       <c r="D23" s="1">
         <v>45718</v>
@@ -1436,11 +2699,11 @@
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
+      <c r="B24">
+        <v>0.160467654466629</v>
+      </c>
+      <c r="C24">
+        <v>0.91250002384185702</v>
       </c>
       <c r="D24" s="1">
         <v>45718</v>
@@ -1453,11 +2716,11 @@
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" t="s">
-        <v>35</v>
+      <c r="B25">
+        <v>0.104829668998718</v>
+      </c>
+      <c r="C25">
+        <v>0.95833331346511796</v>
       </c>
       <c r="D25" s="1">
         <v>45718</v>
@@ -1470,11 +2733,11 @@
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" t="s">
-        <v>37</v>
+      <c r="B26">
+        <v>7.5517028570175102E-2</v>
+      </c>
+      <c r="C26">
+        <v>0.97500002384185702</v>
       </c>
       <c r="D26" s="1">
         <v>45718</v>
@@ -1487,11 +2750,11 @@
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" t="s">
-        <v>39</v>
+      <c r="B27">
+        <v>3.0826391652226399E-2</v>
+      </c>
+      <c r="C27">
+        <v>0.98333334922790505</v>
       </c>
       <c r="D27" s="1">
         <v>45718</v>
@@ -1504,11 +2767,11 @@
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" t="s">
-        <v>41</v>
+      <c r="B28">
+        <v>8.1651927903294494E-3</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
       </c>
       <c r="D28" s="1">
         <v>45718</v>
@@ -1521,11 +2784,11 @@
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" t="s">
-        <v>43</v>
+      <c r="B29">
+        <v>3.3920343965291901E-2</v>
+      </c>
+      <c r="C29">
+        <v>0.98750001192092896</v>
       </c>
       <c r="D29" s="1">
         <v>45718</v>
@@ -1538,11 +2801,11 @@
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" t="s">
-        <v>45</v>
+      <c r="B30">
+        <v>0.160044580698013</v>
+      </c>
+      <c r="C30">
+        <v>0.92083334922790505</v>
       </c>
       <c r="D30" s="1">
         <v>45718</v>
@@ -1555,11 +2818,11 @@
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" t="s">
-        <v>45</v>
+      <c r="B31">
+        <v>0.28659075498580899</v>
+      </c>
+      <c r="C31">
+        <v>0.92083334922790505</v>
       </c>
       <c r="D31" s="1">
         <v>45718</v>
@@ -1570,5 +2833,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aktualisiere Modellpfad, bereinige nicht verwendeten Code und passe Bildverarbeitung an
</commit_message>
<xml_diff>
--- a/Model_Doku_Master_STA2.xlsx
+++ b/Model_Doku_Master_STA2.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\DHBWMA_HHAT_Image-Classification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreasbraig/Documents/VSCode/DHBWMA_HHAT_Image-Classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6A831E-C970-4C6A-A1F7-40A152F87F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C0CFB9-F211-6443-A358-E9404F6A20F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D564533F-BAE4-C643-AF37-CB06E8464E9E}"/>
+    <workbookView xWindow="4080" yWindow="500" windowWidth="30240" windowHeight="17760" activeTab="1" xr2:uid="{D564533F-BAE4-C643-AF37-CB06E8464E9E}"/>
   </bookViews>
   <sheets>
     <sheet name="model30_NEWNET" sheetId="1" r:id="rId1"/>
+    <sheet name="Alle" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
   <si>
     <t>epoch</t>
   </si>
@@ -72,12 +73,24 @@
   <si>
     <t>weighted avg</t>
   </si>
+  <si>
+    <t>Custom CNN Pytorch</t>
+  </si>
+  <si>
+    <t>Mobilenet v3 Tensorflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recall </t>
+  </si>
+  <si>
+    <t>Mobilenet v1 Tensorflow</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -554,10 +567,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1378,7 +1394,618 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Alle!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mobilenet v3 Tensorflow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Alle!$B$2,Alle!$B$12,Alle!$B$22)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Custom CNN Pytorch</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mobilenet v3 Tensorflow</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mobilenet v1 Tensorflow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Alle!$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-08E8-F34C-B9B9-528455C5C626}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Alle!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Custom CNN Pytorch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Alle!$B$2,Alle!$B$12,Alle!$B$22)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Custom CNN Pytorch</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mobilenet v3 Tensorflow</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mobilenet v1 Tensorflow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Alle!$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-08E8-F34C-B9B9-528455C5C626}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Alle!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mobilenet v1 Tensorflow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Alle!$B$2,Alle!$B$12,Alle!$B$22)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Custom CNN Pytorch</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mobilenet v3 Tensorflow</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mobilenet v1 Tensorflow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Alle!$E$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-08E8-F34C-B9B9-528455C5C626}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="857988208"/>
+        <c:axId val="918514544"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="857988208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="918514544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="918514544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="857988208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1934,6 +2561,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1955,6 +3085,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5768AE0-1B80-2D3A-E203-8CCA710185AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B25A5894-AD4F-16AD-5AEA-39B5687EA3C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2294,20 +3465,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50263B4-DD00-C44E-8074-4A680FFC1D62}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32:K39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2324,7 +3495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2341,7 +3512,7 @@
         <v>0.74194444444444441</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2358,7 +3529,7 @@
         <v>0.74237268518518518</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2375,7 +3546,7 @@
         <v>0.74281249999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2392,7 +3563,7 @@
         <v>0.74322916666666672</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2409,7 +3580,7 @@
         <v>0.74366898148148153</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2426,7 +3597,7 @@
         <v>0.74409722222222219</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2443,7 +3614,7 @@
         <v>0.744537037037037</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2460,7 +3631,7 @@
         <v>0.74497685185185181</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2477,7 +3648,7 @@
         <v>0.74541666666666662</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2494,7 +3665,7 @@
         <v>0.74585648148148154</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2511,7 +3682,7 @@
         <v>0.74627314814814816</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2528,7 +3699,7 @@
         <v>0.74668981481481478</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2545,7 +3716,7 @@
         <v>0.74714120370370374</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2562,7 +3733,7 @@
         <v>0.74759259259259259</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2579,7 +3750,7 @@
         <v>0.74805555555555558</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2596,7 +3767,7 @@
         <v>0.74850694444444443</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2613,7 +3784,7 @@
         <v>0.7489351851851852</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2630,7 +3801,7 @@
         <v>0.74938657407407405</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2647,7 +3818,7 @@
         <v>0.74983796296296301</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2664,7 +3835,7 @@
         <v>0.75027777777777782</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2681,7 +3852,7 @@
         <v>0.75070601851851848</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2698,7 +3869,7 @@
         <v>0.75113425925925925</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2715,7 +3886,7 @@
         <v>0.75156250000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2732,7 +3903,7 @@
         <v>0.75199074074074079</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2749,7 +3920,7 @@
         <v>0.75241898148148145</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2766,7 +3937,7 @@
         <v>0.75293981481481487</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2783,19 +3954,19 @@
         <v>0.75342592592592594</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D29" s="1"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D30" s="1"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D31" s="1"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H32" t="s">
         <v>4</v>
       </c>
@@ -2809,7 +3980,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="7:11">
+    <row r="34" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G34" t="s">
         <v>8</v>
       </c>
@@ -2826,7 +3997,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="7:11">
+    <row r="35" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G35" t="s">
         <v>12</v>
       </c>
@@ -2843,7 +4014,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="7:11">
+    <row r="37" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G37" t="s">
         <v>14</v>
       </c>
@@ -2854,7 +4025,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="7:11">
+    <row r="38" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G38" t="s">
         <v>15</v>
       </c>
@@ -2871,7 +4042,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="7:11">
+    <row r="39" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G39" t="s">
         <v>16</v>
       </c>
@@ -2892,4 +4063,337 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795FFA63-5DB0-4B4B-881B-191AF4D3AF1A}">
+  <dimension ref="B2:F30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0.96</v>
+      </c>
+      <c r="E5">
+        <v>0.98</v>
+      </c>
+      <c r="F5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>0.97</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0.98</v>
+      </c>
+      <c r="F6">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>0.98</v>
+      </c>
+      <c r="F8">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>0.98</v>
+      </c>
+      <c r="D9">
+        <v>0.98</v>
+      </c>
+      <c r="E9">
+        <v>0.98</v>
+      </c>
+      <c r="F9">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>0.98</v>
+      </c>
+      <c r="D10">
+        <v>0.98</v>
+      </c>
+      <c r="E10">
+        <v>0.98</v>
+      </c>
+      <c r="F10">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>0.44</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0.61</v>
+      </c>
+      <c r="F15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18">
+        <v>0.44</v>
+      </c>
+      <c r="F18">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>0.22</v>
+      </c>
+      <c r="D19">
+        <v>0.5</v>
+      </c>
+      <c r="E19">
+        <v>0.3</v>
+      </c>
+      <c r="F19">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>0.19</v>
+      </c>
+      <c r="D20">
+        <v>0.44</v>
+      </c>
+      <c r="E20">
+        <v>0.27</v>
+      </c>
+      <c r="F20">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>0.87</v>
+      </c>
+      <c r="D25">
+        <v>0.72</v>
+      </c>
+      <c r="E25">
+        <v>0.79</v>
+      </c>
+      <c r="F25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26">
+        <v>0.81</v>
+      </c>
+      <c r="D26">
+        <v>0.92</v>
+      </c>
+      <c r="E26">
+        <v>0.86</v>
+      </c>
+      <c r="F26">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28">
+        <v>0.83</v>
+      </c>
+      <c r="F28">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29">
+        <v>0.84</v>
+      </c>
+      <c r="D29">
+        <v>0.82</v>
+      </c>
+      <c r="E29">
+        <v>0.82</v>
+      </c>
+      <c r="F29">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <v>0.83</v>
+      </c>
+      <c r="D30">
+        <v>0.83</v>
+      </c>
+      <c r="E30">
+        <v>0.83</v>
+      </c>
+      <c r="F30">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B22:F22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{d792d246-d363-40e2-82bc-6f0655128b68}" enabled="1" method="Standard" siteId="{372ee9e0-9ce0-4033-a64a-c07073a91ecd}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Aktualisiere binäre Dateien und entferne temporäre Excel-Datei
</commit_message>
<xml_diff>
--- a/Model_Doku_Master_STA2.xlsx
+++ b/Model_Doku_Master_STA2.xlsx
@@ -8,14 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreasbraig/Documents/VSCode/DHBWMA_HHAT_Image-Classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C0CFB9-F211-6443-A358-E9404F6A20F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451AFC0F-2B5B-0F40-BAEE-9ACB10B79876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="500" windowWidth="30240" windowHeight="17760" activeTab="1" xr2:uid="{D564533F-BAE4-C643-AF37-CB06E8464E9E}"/>
+    <workbookView xWindow="-40840" yWindow="1000" windowWidth="36020" windowHeight="23400" activeTab="1" xr2:uid="{D564533F-BAE4-C643-AF37-CB06E8464E9E}"/>
   </bookViews>
   <sheets>
     <sheet name="model30_NEWNET" sheetId="1" r:id="rId1"/>
     <sheet name="Alle" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">(Alle!$B$2,Alle!$B$12,Alle!$B$22)</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Alle!$B$12</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Alle!$B$22</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Alle!$E$18</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Alle!$E$28</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Alle!$E$8</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Alle!$B$2</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Alle!$B$22</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Alle!$E$18</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Alle!$E$28</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Alle!$E$8</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">(Alle!$B$2,Alle!$B$12,Alle!$B$22)</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Alle!$B$12</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Alle!$B$2</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1394,618 +1410,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Alle!$B$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Mobilenet v3 Tensorflow</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>(Alle!$B$2,Alle!$B$12,Alle!$B$22)</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Custom CNN Pytorch</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Mobilenet v3 Tensorflow</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Mobilenet v1 Tensorflow</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Alle!$E$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.44</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-08E8-F34C-B9B9-528455C5C626}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Alle!$B$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Custom CNN Pytorch</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>(Alle!$B$2,Alle!$B$12,Alle!$B$22)</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Custom CNN Pytorch</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Mobilenet v3 Tensorflow</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Mobilenet v1 Tensorflow</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Alle!$E$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.98</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-08E8-F34C-B9B9-528455C5C626}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Alle!$B$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Mobilenet v1 Tensorflow</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>(Alle!$B$2,Alle!$B$12,Alle!$B$22)</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Custom CNN Pytorch</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Mobilenet v3 Tensorflow</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Mobilenet v1 Tensorflow</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Alle!$E$28</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.83</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-08E8-F34C-B9B9-528455C5C626}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="857988208"/>
-        <c:axId val="918514544"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="857988208"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="918514544"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="918514544"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="857988208"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2561,509 +1966,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3085,47 +1987,6 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5768AE0-1B80-2D3A-E203-8CCA710185AA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B25A5894-AD4F-16AD-5AEA-39B5687EA3C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4070,7 +2931,7 @@
   <dimension ref="B2:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4388,7 +3249,6 @@
     <mergeCell ref="B22:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>